<commit_message>
Actualización: añadí nuevos datos de entrenamiento y pruebas
</commit_message>
<xml_diff>
--- a/uploads/prediction/resultados_prediccion.xlsx
+++ b/uploads/prediction/resultados_prediccion.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>81.42</v>
+        <v>80.86</v>
       </c>
     </row>
     <row r="3">
@@ -488,7 +488,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>83.69</v>
+        <v>83.25</v>
       </c>
     </row>
     <row r="4">
@@ -502,11 +502,11 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Aprobado</t>
+          <t>Desaprobado</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>56.92</v>
+        <v>45.68</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>35.53</v>
+        <v>26.73</v>
       </c>
     </row>
     <row r="6">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>60.54</v>
+        <v>51.8</v>
       </c>
     </row>
     <row r="7">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>66.76000000000001</v>
+        <v>58.38</v>
       </c>
     </row>
     <row r="8">
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>63.61</v>
+        <v>54.03</v>
       </c>
     </row>
     <row r="9">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>59.1</v>
+        <v>50.26</v>
       </c>
     </row>
     <row r="10">
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>69.34999999999999</v>
+        <v>62.45</v>
       </c>
     </row>
     <row r="11">
@@ -628,11 +628,11 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Aprobado</t>
+          <t>Desaprobado</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>54.76</v>
+        <v>45.71</v>
       </c>
     </row>
     <row r="12">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>65.98999999999999</v>
+        <v>57.17</v>
       </c>
     </row>
     <row r="13">
@@ -664,11 +664,11 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Aprobado</t>
+          <t>Desaprobado</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>54.04</v>
+        <v>42.94</v>
       </c>
     </row>
     <row r="14">
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>64.09999999999999</v>
+        <v>55.86</v>
       </c>
     </row>
     <row r="15">
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>60.67</v>
+        <v>50.87</v>
       </c>
     </row>
     <row r="16">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>60.26</v>
+        <v>50.29</v>
       </c>
     </row>
     <row r="17">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>33.33</v>
+        <v>23.84</v>
       </c>
     </row>
     <row r="18">
@@ -754,11 +754,11 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Aprobado</t>
+          <t>Desaprobado</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>54.33</v>
+        <v>45.22</v>
       </c>
     </row>
     <row r="19">
@@ -772,11 +772,11 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Aprobado</t>
+          <t>Desaprobado</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>55.51</v>
+        <v>45.16</v>
       </c>
     </row>
     <row r="20">
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>61.72</v>
+        <v>51.89</v>
       </c>
     </row>
     <row r="21">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>76.23999999999999</v>
+        <v>72.09999999999999</v>
       </c>
     </row>
     <row r="22">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>64.09999999999999</v>
+        <v>55.86</v>
       </c>
     </row>
     <row r="23">
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>79.31</v>
+        <v>73.56</v>
       </c>
     </row>
     <row r="24">
@@ -866,7 +866,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>77.25</v>
+        <v>72.54000000000001</v>
       </c>
     </row>
     <row r="25">
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>76.78</v>
+        <v>70.83</v>
       </c>
     </row>
     <row r="26">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>48.62</v>
+        <v>39.39</v>
       </c>
     </row>
     <row r="27">
@@ -920,7 +920,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>39.89</v>
+        <v>29.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>